<commit_message>
- added more user stories and updated their status;
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Requirements Engineering</t>
   </si>
@@ -978,6 +978,52 @@
         <scheme val="minor"/>
       </rPr>
       <t>. Assign any project to any team supervisor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">USID 42 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. See a report history on the tasks I created so I can better visualize the project's state.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USID 43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. To choose whether the alarm will be a notification tray pop-up, or a classic pop-up with or without sound.</t>
     </r>
   </si>
 </sst>
@@ -1054,14 +1100,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,39 +1422,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="36.6" x14ac:dyDescent="0.7">
       <c r="I2" s="2"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="5"/>
+      <c r="A3" s="3"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -1617,6 +1663,16 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updated the user stories with the latest things; - this commit should hold all the base user stories necessary to advance to the next step, and all further commits here should only ADD additional functions, not critical ones;
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g0dzax\Documents\Tracker\trackerUserStories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tracker\trackerUserStories\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUS" sheetId="1" r:id="rId1"/>
@@ -26,26 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="158">
-  <si>
-    <t>Requirements Engineering</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="158">
   <si>
     <t>As a user, I want to be able to:</t>
   </si>
   <si>
-    <t xml:space="preserve">   I.</t>
-  </si>
-  <si>
     <t>I.1 - General User stories</t>
   </si>
   <si>
     <t>I.2 - Objective User stories</t>
   </si>
   <si>
-    <t>I.3 - Task User stories</t>
-  </si>
-  <si>
     <t>OUS 1.</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
     <t>GUS 2.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Create my own widgets that will display whatever information I select.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 3. </t>
   </si>
   <si>
@@ -73,9 +61,6 @@
     <t>GUS 4.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Set any permissions I want to any member of a team.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 5. </t>
   </si>
   <si>
@@ -118,9 +103,6 @@
     <t>GUS 12.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Manage one task in a graphical, structured view that will display all the details related to that task.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 13. </t>
   </si>
   <si>
@@ -136,15 +118,9 @@
     <t>GUS 15.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Assing any task to any project.</t>
-  </si>
-  <si>
     <t>GUS 16.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Assign any team member to any task.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 17. </t>
   </si>
   <si>
@@ -154,9 +130,6 @@
     <t>GUS 18.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Set an alarm timer for any project or task or team member.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 19. </t>
   </si>
   <si>
@@ -202,9 +175,6 @@
     <t>GUS 26.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Assign tasks to myself.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 27. </t>
   </si>
   <si>
@@ -268,9 +238,6 @@
     <t>GUS 37.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Send requests for the supervisor to check my accomplished tasks.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 38. </t>
   </si>
   <si>
@@ -280,15 +247,9 @@
     <t>GUS 39.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Be confident in the fact that my data is secured and encrypted.</t>
-  </si>
-  <si>
     <t>GUS 40.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Use a manual that guies me on how to use the application.</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUS 41. </t>
   </si>
   <si>
@@ -298,15 +259,9 @@
     <t>GUS 42 .</t>
   </si>
   <si>
-    <t xml:space="preserve"> See a report history on the tasks I created so I can better visualize the project's state.</t>
-  </si>
-  <si>
     <t>GUS 43.</t>
   </si>
   <si>
-    <t xml:space="preserve"> To choose whether the alarm will be a notification tray pop-up, or a classic pop-up with or without sound.</t>
-  </si>
-  <si>
     <t>Set a title.</t>
   </si>
   <si>
@@ -500,6 +455,51 @@
   </si>
   <si>
     <t>Manage all my tasks in a graphical, structured view.</t>
+  </si>
+  <si>
+    <t>I. Requirements Engineering</t>
+  </si>
+  <si>
+    <t>I.Requirements Engineering</t>
+  </si>
+  <si>
+    <t>I.2 - Task User stories</t>
+  </si>
+  <si>
+    <t>Assing any task to any project.</t>
+  </si>
+  <si>
+    <t>Assign any team member to any task.</t>
+  </si>
+  <si>
+    <t>Set an alarm timer for any project or task or team member.</t>
+  </si>
+  <si>
+    <t>Assign tasks to myself.</t>
+  </si>
+  <si>
+    <t>Send requests for the supervisor to check my accomplished tasks.</t>
+  </si>
+  <si>
+    <t>Be confident in the fact that my data is secured and encrypted.</t>
+  </si>
+  <si>
+    <t>Use a manual that guies me on how to use the application.</t>
+  </si>
+  <si>
+    <t>See a report history on the tasks I created so I can better visualize the project's state.</t>
+  </si>
+  <si>
+    <t>To choose whether the alarm will be a notification tray pop-up, or a classic pop-up with or without sound.</t>
+  </si>
+  <si>
+    <t>Create my own widgets that will display whatever information I select.</t>
+  </si>
+  <si>
+    <t>Set any permissions I want to any member of a team.</t>
+  </si>
+  <si>
+    <t>Manage one task in a graphical, structured view that will display all the details related to that task.</t>
   </si>
 </sst>
 </file>
@@ -530,13 +530,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="28"/>
       <color theme="1"/>
@@ -544,6 +537,14 @@
       <family val="1"/>
     </font>
     <font>
+      <i/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="28"/>
       <color theme="1"/>
@@ -571,28 +572,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,391 +911,407 @@
   </sheetPr>
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="G2" s="9"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B39" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="B41" t="s">
         <v>71</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="B44" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1307,192 +1322,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="G2" s="9"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>6</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>154</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1502,198 +1533,214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="G2" s="9"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>133</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>